<commit_message>
Update Data Attribute Description File.xlsx
</commit_message>
<xml_diff>
--- a/data/Data Attribute Description File.xlsx
+++ b/data/Data Attribute Description File.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justi\Documents\GitHub\olist\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D61D9AF0-8E0E-4A91-B327-733FFF1579AA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF3A8DD3-E149-45EB-BD1F-A4C8D91AA4ED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28080" windowHeight="16440" activeTab="1" xr2:uid="{DE0F9616-EF0B-4A6C-BB48-F9C91E36FA78}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28080" windowHeight="16440" xr2:uid="{DE0F9616-EF0B-4A6C-BB48-F9C91E36FA78}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Attributes Initial Load" sheetId="1" r:id="rId1"/>
     <sheet name="Missing Data Pass 1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="93">
   <si>
     <t>order_id</t>
   </si>
@@ -166,12 +166,6 @@
     <t>review_answer_timestamp</t>
   </si>
   <si>
-    <t>purchase_wk_day</t>
-  </si>
-  <si>
-    <t>purchase_month</t>
-  </si>
-  <si>
     <t>attribute</t>
   </si>
   <si>
@@ -232,9 +226,6 @@
     <t>number of payment methods used by the customer</t>
   </si>
   <si>
-    <t>method of payment by customer</t>
-  </si>
-  <si>
     <t>number of payment installments by customer</t>
   </si>
   <si>
@@ -247,36 +238,18 @@
     <t>comment titles from the review left by the customer</t>
   </si>
   <si>
-    <t>comment message from the review left by the customer</t>
-  </si>
-  <si>
     <t>date satisfaction survey sent to customer</t>
   </si>
   <si>
     <t>satisfaction survey answer timestamp</t>
   </si>
   <si>
-    <t>weekday name purchase was initiated</t>
-  </si>
-  <si>
-    <t>month name purchase was initiated</t>
-  </si>
-  <si>
     <t>order status, 7-levels (shipped, canceled, invoiced, processing, approved, unavailable, delivered)</t>
   </si>
   <si>
     <t>purchase initiation timestamp</t>
   </si>
   <si>
-    <t>payment approval timestamp</t>
-  </si>
-  <si>
-    <t>order posting timestamp when it was handed to the logistic partner</t>
-  </si>
-  <si>
-    <t>actual order delivery date to the customer</t>
-  </si>
-  <si>
     <t>estimated delivery date provided to the customer at the time of purchase initiation</t>
   </si>
   <si>
@@ -308,13 +281,46 @@
   </si>
   <si>
     <t>NaN</t>
+  </si>
+  <si>
+    <t>method of payment by customer [74% credit_card, 19% boleto, 7% other]</t>
+  </si>
+  <si>
+    <t>comment message from the review left by the customer [note: 58% missing]</t>
+  </si>
+  <si>
+    <t>Missing Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">order posting timestamp when it was handed to the logistic partner </t>
+  </si>
+  <si>
+    <t xml:space="preserve">actual order delivery date to the customer </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2% = 1,783</t>
+  </si>
+  <si>
+    <t>3% = 2,965</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2% = 610 </t>
+  </si>
+  <si>
+    <t>88% = 88.3K</t>
+  </si>
+  <si>
+    <t>58%=58.2k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">payment approval timestamp </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -342,6 +348,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -363,7 +377,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -371,6 +385,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -686,31 +707,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D01C5B58-AB22-460E-901C-01A059B8C06B}">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="C43" sqref="A1:C43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="91.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="79.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -718,10 +743,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -729,10 +757,13 @@
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -740,10 +771,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -751,10 +785,13 @@
         <v>5</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -762,10 +799,13 @@
         <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+      <c r="D6" s="4">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -773,10 +813,13 @@
         <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
@@ -784,10 +827,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
@@ -795,10 +841,13 @@
         <v>5</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
@@ -806,10 +855,13 @@
         <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
@@ -817,10 +869,13 @@
         <v>1</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
@@ -828,10 +883,13 @@
         <v>1</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
@@ -839,10 +897,13 @@
         <v>1</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
@@ -850,10 +911,13 @@
         <v>1</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="D14" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>15</v>
       </c>
@@ -861,10 +925,13 @@
         <v>1</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="D15" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>16</v>
       </c>
@@ -872,10 +939,13 @@
         <v>1</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="D16" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>17</v>
       </c>
@@ -883,10 +953,13 @@
         <v>5</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="D17" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>18</v>
       </c>
@@ -894,10 +967,13 @@
         <v>19</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="D18" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>20</v>
       </c>
@@ -905,10 +981,13 @@
         <v>19</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="D19" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>21</v>
       </c>
@@ -916,10 +995,13 @@
         <v>19</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="D20" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>22</v>
       </c>
@@ -927,10 +1009,13 @@
         <v>1</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+      <c r="D21" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>23</v>
       </c>
@@ -938,10 +1023,13 @@
         <v>19</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="D22" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>24</v>
       </c>
@@ -949,10 +1037,13 @@
         <v>19</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="D23" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>25</v>
       </c>
@@ -960,10 +1051,13 @@
         <v>1</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="D24" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>26</v>
       </c>
@@ -971,10 +1065,13 @@
         <v>1</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="D25" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>27</v>
       </c>
@@ -982,10 +1079,13 @@
         <v>1</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="D26" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>28</v>
       </c>
@@ -993,10 +1093,13 @@
         <v>1</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>29</v>
       </c>
@@ -1004,10 +1107,13 @@
         <v>19</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>30</v>
       </c>
@@ -1015,10 +1121,13 @@
         <v>19</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>31</v>
       </c>
@@ -1026,10 +1135,13 @@
         <v>19</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>32</v>
       </c>
@@ -1037,10 +1149,13 @@
         <v>19</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="D31" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>33</v>
       </c>
@@ -1048,10 +1163,13 @@
         <v>19</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+      <c r="D32" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>34</v>
       </c>
@@ -1059,10 +1177,13 @@
         <v>19</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="D33" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>35</v>
       </c>
@@ -1070,10 +1191,13 @@
         <v>19</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="D34" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>36</v>
       </c>
@@ -1081,10 +1205,13 @@
         <v>1</v>
       </c>
       <c r="C35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D35" s="4" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>37</v>
       </c>
@@ -1092,10 +1219,13 @@
         <v>1</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="D36" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>38</v>
       </c>
@@ -1103,10 +1233,13 @@
         <v>19</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="D37" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>39</v>
       </c>
@@ -1114,10 +1247,13 @@
         <v>1</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>40</v>
       </c>
@@ -1125,10 +1261,13 @@
         <v>1</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>41</v>
       </c>
@@ -1136,10 +1275,13 @@
         <v>5</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="D40" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>42</v>
       </c>
@@ -1147,30 +1289,21 @@
         <v>5</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>74</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="D41" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="3"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="3"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1182,7 +1315,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FDC8B4F-7E0E-4857-BD15-EE4ECD2786DD}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B10"/>
     </sheetView>
   </sheetViews>
@@ -1193,10 +1326,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B1" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updates and new files
* added the summary table to the data attribute desc file
* adding in the summary table as a csv
* updated my python code to dive into what might be outliers
</commit_message>
<xml_diff>
--- a/data/Data Attribute Description File.xlsx
+++ b/data/Data Attribute Description File.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justi\Documents\GitHub\olist\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDFE00D8-6BC8-4F64-B727-E9A7CDAB1616}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF0DBF0A-B873-4C53-A9BB-19740A9A1E29}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27990" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="3" xr2:uid="{DE0F9616-EF0B-4A6C-BB48-F9C91E36FA78}"/>
+    <workbookView xWindow="-27990" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="4" xr2:uid="{DE0F9616-EF0B-4A6C-BB48-F9C91E36FA78}"/>
   </bookViews>
   <sheets>
     <sheet name="Merge" sheetId="3" r:id="rId1"/>
     <sheet name="Attributes Initial Load" sheetId="1" r:id="rId2"/>
     <sheet name="Missing Data Pass 1" sheetId="2" r:id="rId3"/>
     <sheet name="Column Names" sheetId="4" r:id="rId4"/>
+    <sheet name="Olist_Variable_Descriptions" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="155">
   <si>
     <t>order_id</t>
   </si>
@@ -424,6 +425,84 @@
   </si>
   <si>
     <t>product_category_english</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>std</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>last</t>
+  </si>
+  <si>
+    <t>first</t>
+  </si>
+  <si>
+    <t>freq</t>
+  </si>
+  <si>
+    <t>August</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>SP</t>
+  </si>
+  <si>
+    <t>sao paulo</t>
+  </si>
+  <si>
+    <t>bed_bath_table</t>
+  </si>
+  <si>
+    <t>4a3ca9315b744ce9f8e9374361493884</t>
+  </si>
+  <si>
+    <t>aca2eb7d00ea1a7b8ebd4e68314663af</t>
+  </si>
+  <si>
+    <t>credit_card</t>
+  </si>
+  <si>
+    <t>Muito bom</t>
+  </si>
+  <si>
+    <t>Recomendo</t>
+  </si>
+  <si>
+    <t>eef5dbca8d37dfce6db7d7b16dd0525e</t>
+  </si>
+  <si>
+    <t>9a736b248f67d166d2fbb006bcb877c3</t>
+  </si>
+  <si>
+    <t>270c23a11d024a44c896d1894b261a83</t>
+  </si>
+  <si>
+    <t>895ab968e7bb0d5659d16cd74cd1650c</t>
+  </si>
+  <si>
+    <t>top</t>
+  </si>
+  <si>
+    <t>unique</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>purchase_month</t>
+  </si>
+  <si>
+    <t>purchase_wk_day</t>
   </si>
 </sst>
 </file>
@@ -518,7 +597,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -552,6 +631,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1991,8 +2076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7257E28C-A4CB-4D7E-8AC1-34D45E3E0C74}">
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25:D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2029,7 +2114,7 @@
         <v>118</v>
       </c>
       <c r="H1" t="b">
-        <f>B1=D1</f>
+        <f t="shared" ref="H1:H39" si="0">B1=D1</f>
         <v>1</v>
       </c>
     </row>
@@ -2056,7 +2141,7 @@
         <v>118</v>
       </c>
       <c r="H2" t="b">
-        <f>B2=D2</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2083,7 +2168,7 @@
         <v>118</v>
       </c>
       <c r="H3" t="b">
-        <f>B3=D3</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2110,7 +2195,7 @@
         <v>118</v>
       </c>
       <c r="H4" t="b">
-        <f>B4=D4</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2137,7 +2222,7 @@
         <v>119</v>
       </c>
       <c r="H5" t="b">
-        <f>B5=D5</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2164,7 +2249,7 @@
         <v>19</v>
       </c>
       <c r="H6" t="b">
-        <f>B6=D6</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2191,7 +2276,7 @@
         <v>118</v>
       </c>
       <c r="H7" t="b">
-        <f>B7=D7</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2218,7 +2303,7 @@
         <v>118</v>
       </c>
       <c r="H8" t="b">
-        <f>B8=D8</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2245,7 +2330,7 @@
         <v>118</v>
       </c>
       <c r="H9" t="b">
-        <f>B9=D9</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2272,7 +2357,7 @@
         <v>118</v>
       </c>
       <c r="H10" t="b">
-        <f>B10=D10</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2299,7 +2384,7 @@
         <v>118</v>
       </c>
       <c r="H11" t="b">
-        <f>B11=D11</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2326,7 +2411,7 @@
         <v>19</v>
       </c>
       <c r="H12" t="b">
-        <f>B12=D12</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2353,7 +2438,7 @@
         <v>118</v>
       </c>
       <c r="H13" t="b">
-        <f>B13=D13</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2380,7 +2465,7 @@
         <v>118</v>
       </c>
       <c r="H14" t="b">
-        <f>B14=D14</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2407,7 +2492,7 @@
         <v>119</v>
       </c>
       <c r="H15" t="b">
-        <f>B15=D15</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2434,7 +2519,7 @@
         <v>119</v>
       </c>
       <c r="H16" t="b">
-        <f>B16=D16</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2461,7 +2546,7 @@
         <v>118</v>
       </c>
       <c r="H17" t="b">
-        <f>B17=D17</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2488,7 +2573,7 @@
         <v>19</v>
       </c>
       <c r="H18" t="b">
-        <f>B18=D18</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2515,7 +2600,7 @@
         <v>19</v>
       </c>
       <c r="H19" t="b">
-        <f>B19=D19</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2542,7 +2627,7 @@
         <v>118</v>
       </c>
       <c r="H20" t="b">
-        <f>B20=D20</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2569,7 +2654,7 @@
         <v>19</v>
       </c>
       <c r="H21" t="b">
-        <f>B21=D21</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2596,7 +2681,7 @@
         <v>19</v>
       </c>
       <c r="H22" t="b">
-        <f>B22=D22</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2623,7 +2708,7 @@
         <v>118</v>
       </c>
       <c r="H23" t="b">
-        <f>B23=D23</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2650,7 +2735,7 @@
         <v>19</v>
       </c>
       <c r="H24" t="b">
-        <f>B24=D24</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2677,7 +2762,7 @@
         <v>19</v>
       </c>
       <c r="H25" t="b">
-        <f>B25=D25</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2704,7 +2789,7 @@
         <v>19</v>
       </c>
       <c r="H26" t="b">
-        <f>B26=D26</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2731,7 +2816,7 @@
         <v>19</v>
       </c>
       <c r="H27" t="b">
-        <f>B27=D27</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2758,7 +2843,7 @@
         <v>19</v>
       </c>
       <c r="H28" t="b">
-        <f>B28=D28</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2785,7 +2870,7 @@
         <v>118</v>
       </c>
       <c r="H29" t="b">
-        <f>B29=D29</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2812,7 +2897,7 @@
         <v>118</v>
       </c>
       <c r="H30" t="b">
-        <f>B30=D30</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2839,7 +2924,7 @@
         <v>118</v>
       </c>
       <c r="H31" t="b">
-        <f>B31=D31</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2866,7 +2951,7 @@
         <v>118</v>
       </c>
       <c r="H32" t="b">
-        <f>B32=D32</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2893,7 +2978,7 @@
         <v>118</v>
       </c>
       <c r="H33" t="b">
-        <f>B33=D33</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2920,7 +3005,7 @@
         <v>119</v>
       </c>
       <c r="H34" t="b">
-        <f>B34=D34</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2947,7 +3032,7 @@
         <v>118</v>
       </c>
       <c r="H35" t="b">
-        <f>B35=D35</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2974,7 +3059,7 @@
         <v>118</v>
       </c>
       <c r="H36" t="b">
-        <f>B36=D36</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3001,7 +3086,7 @@
         <v>118</v>
       </c>
       <c r="H37" t="b">
-        <f>B37=D37</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3028,7 +3113,7 @@
         <v>19</v>
       </c>
       <c r="H38" t="b">
-        <f>B38=D38</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3055,7 +3140,7 @@
         <v>118</v>
       </c>
       <c r="H39" t="b">
-        <f>B39=D39</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3066,4 +3151,936 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95DF7814-38F0-41B9-A485-5DC01AD93DEF}">
+  <dimension ref="A1:AO14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="AB2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="AF28" sqref="AF28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="34" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="35" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="25.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14" style="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="21.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="34.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="33.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19" style="5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12" style="5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="20.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="26.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="19.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="17.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="33" max="34" width="18.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="17.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="24.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="21.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="10.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="11.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="16.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="16" style="5" bestFit="1" customWidth="1"/>
+    <col min="42" max="16384" width="9.140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="W1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="AB1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="AC1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="AE1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AF1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="AG1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="AH1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="AI1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AJ1" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="AK1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="AL1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="AM1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="AN1" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="AO1" s="5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="B2" s="5">
+        <v>114081</v>
+      </c>
+      <c r="C2" s="5">
+        <v>114081</v>
+      </c>
+      <c r="D2" s="5">
+        <v>114081</v>
+      </c>
+      <c r="E2" s="5">
+        <v>114081</v>
+      </c>
+      <c r="F2" s="5">
+        <v>114080</v>
+      </c>
+      <c r="G2" s="5">
+        <v>114081</v>
+      </c>
+      <c r="H2" s="5">
+        <v>114081</v>
+      </c>
+      <c r="I2" s="5">
+        <v>114081</v>
+      </c>
+      <c r="J2" s="5">
+        <v>114081</v>
+      </c>
+      <c r="K2" s="5">
+        <v>114081</v>
+      </c>
+      <c r="L2" s="5">
+        <v>114081</v>
+      </c>
+      <c r="M2" s="5">
+        <v>114081</v>
+      </c>
+      <c r="N2" s="5">
+        <v>114081</v>
+      </c>
+      <c r="O2" s="5">
+        <v>13667</v>
+      </c>
+      <c r="P2" s="5">
+        <v>48227</v>
+      </c>
+      <c r="Q2" s="5">
+        <v>114081</v>
+      </c>
+      <c r="R2" s="5">
+        <v>114081</v>
+      </c>
+      <c r="S2" s="5">
+        <v>114081</v>
+      </c>
+      <c r="T2" s="5">
+        <v>114081</v>
+      </c>
+      <c r="U2" s="5">
+        <v>114081</v>
+      </c>
+      <c r="V2" s="5">
+        <v>114081</v>
+      </c>
+      <c r="W2" s="5">
+        <v>114081</v>
+      </c>
+      <c r="X2" s="5">
+        <v>114081</v>
+      </c>
+      <c r="Y2" s="5">
+        <v>114081</v>
+      </c>
+      <c r="Z2" s="5">
+        <v>114081</v>
+      </c>
+      <c r="AA2" s="5">
+        <v>114081</v>
+      </c>
+      <c r="AB2" s="5">
+        <v>114081</v>
+      </c>
+      <c r="AC2" s="5">
+        <v>114081</v>
+      </c>
+      <c r="AD2" s="5">
+        <v>114081</v>
+      </c>
+      <c r="AE2" s="5">
+        <v>114081</v>
+      </c>
+      <c r="AF2" s="5">
+        <v>114081</v>
+      </c>
+      <c r="AG2" s="5">
+        <v>114081</v>
+      </c>
+      <c r="AH2" s="5">
+        <v>114081</v>
+      </c>
+      <c r="AI2" s="5">
+        <v>114081</v>
+      </c>
+      <c r="AJ2" s="5">
+        <v>114081</v>
+      </c>
+      <c r="AK2" s="5">
+        <v>114081</v>
+      </c>
+      <c r="AL2" s="5">
+        <v>114081</v>
+      </c>
+      <c r="AM2" s="5">
+        <v>114081</v>
+      </c>
+      <c r="AN2" s="5">
+        <v>114081</v>
+      </c>
+      <c r="AO2" s="5">
+        <v>114081</v>
+      </c>
+    </row>
+    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B3" s="5">
+        <v>95136</v>
+      </c>
+      <c r="C3" s="5">
+        <v>95136</v>
+      </c>
+      <c r="D3" s="5">
+        <v>94632</v>
+      </c>
+      <c r="E3" s="5">
+        <v>87132</v>
+      </c>
+      <c r="F3" s="5">
+        <v>78925</v>
+      </c>
+      <c r="G3" s="5">
+        <v>94348</v>
+      </c>
+      <c r="H3" s="5">
+        <v>444</v>
+      </c>
+      <c r="I3" s="5">
+        <v>92088</v>
+      </c>
+      <c r="J3" s="5">
+        <v>14844</v>
+      </c>
+      <c r="K3" s="5">
+        <v>4073</v>
+      </c>
+      <c r="L3" s="5">
+        <v>27</v>
+      </c>
+      <c r="M3" s="5">
+        <v>94955</v>
+      </c>
+      <c r="O3" s="5">
+        <v>4409</v>
+      </c>
+      <c r="P3" s="5">
+        <v>34589</v>
+      </c>
+      <c r="Q3" s="5">
+        <v>627</v>
+      </c>
+      <c r="R3" s="5">
+        <v>94808</v>
+      </c>
+      <c r="T3" s="5">
+        <v>4</v>
+      </c>
+      <c r="W3" s="5">
+        <v>21</v>
+      </c>
+      <c r="X3" s="5">
+        <v>31629</v>
+      </c>
+      <c r="Y3" s="5">
+        <v>2914</v>
+      </c>
+      <c r="Z3" s="5">
+        <v>90135</v>
+      </c>
+      <c r="AJ3" s="5">
+        <v>73</v>
+      </c>
+      <c r="AK3" s="5">
+        <v>2136</v>
+      </c>
+      <c r="AL3" s="5">
+        <v>588</v>
+      </c>
+      <c r="AM3" s="5">
+        <v>22</v>
+      </c>
+      <c r="AN3" s="5">
+        <v>7</v>
+      </c>
+      <c r="AO3" s="5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="D4" s="18">
+        <v>42955.851747685185</v>
+      </c>
+      <c r="E4" s="18">
+        <v>42955.863553240742</v>
+      </c>
+      <c r="F4" s="18">
+        <v>42957.498773148145</v>
+      </c>
+      <c r="G4" s="18">
+        <v>42961.532152777778</v>
+      </c>
+      <c r="H4" s="18">
+        <v>43089</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="J4" s="5">
+        <v>24220</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="O4" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q4" s="18">
+        <v>43088</v>
+      </c>
+      <c r="R4" s="18">
+        <v>42964.929108796299</v>
+      </c>
+      <c r="T4" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="W4" s="5">
+        <v>1</v>
+      </c>
+      <c r="X4" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="Y4" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="Z4" s="18">
+        <v>42961.863553240742</v>
+      </c>
+      <c r="AJ4" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AK4" s="5">
+        <v>14940</v>
+      </c>
+      <c r="AL4" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="AM4" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="AN4" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="AO4" s="5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B5" s="5">
+        <v>63</v>
+      </c>
+      <c r="C5" s="5">
+        <v>63</v>
+      </c>
+      <c r="D5" s="5">
+        <v>63</v>
+      </c>
+      <c r="E5" s="5">
+        <v>63</v>
+      </c>
+      <c r="F5" s="5">
+        <v>63</v>
+      </c>
+      <c r="G5" s="5">
+        <v>63</v>
+      </c>
+      <c r="H5" s="5">
+        <v>644</v>
+      </c>
+      <c r="I5" s="5">
+        <v>75</v>
+      </c>
+      <c r="J5" s="5">
+        <v>152</v>
+      </c>
+      <c r="K5" s="5">
+        <v>18002</v>
+      </c>
+      <c r="L5" s="5">
+        <v>48124</v>
+      </c>
+      <c r="M5" s="5">
+        <v>63</v>
+      </c>
+      <c r="O5" s="5">
+        <v>492</v>
+      </c>
+      <c r="P5" s="5">
+        <v>253</v>
+      </c>
+      <c r="Q5" s="5">
+        <v>526</v>
+      </c>
+      <c r="R5" s="5">
+        <v>63</v>
+      </c>
+      <c r="T5" s="5">
+        <v>84177</v>
+      </c>
+      <c r="W5" s="5">
+        <v>99874</v>
+      </c>
+      <c r="X5" s="5">
+        <v>529</v>
+      </c>
+      <c r="Y5" s="5">
+        <v>2116</v>
+      </c>
+      <c r="Z5" s="5">
+        <v>63</v>
+      </c>
+      <c r="AJ5" s="5">
+        <v>11816</v>
+      </c>
+      <c r="AK5" s="5">
+        <v>8196</v>
+      </c>
+      <c r="AL5" s="5">
+        <v>28431</v>
+      </c>
+      <c r="AM5" s="5">
+        <v>81383</v>
+      </c>
+      <c r="AN5" s="5">
+        <v>18551</v>
+      </c>
+      <c r="AO5" s="5">
+        <v>12353</v>
+      </c>
+    </row>
+    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="D6" s="18">
+        <v>42646.406134259261</v>
+      </c>
+      <c r="E6" s="18">
+        <v>42647.405231481483</v>
+      </c>
+      <c r="F6" s="18">
+        <v>42651.440289351849</v>
+      </c>
+      <c r="G6" s="18">
+        <v>42654.573981481481</v>
+      </c>
+      <c r="H6" s="18">
+        <v>42670</v>
+      </c>
+      <c r="Q6" s="18">
+        <v>42658</v>
+      </c>
+      <c r="R6" s="18">
+        <v>42659.139085648145</v>
+      </c>
+      <c r="Z6" s="18">
+        <v>42651.440289351849</v>
+      </c>
+    </row>
+    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D7" s="18">
+        <v>43341.625428240739</v>
+      </c>
+      <c r="E7" s="18">
+        <v>43341.632245370369</v>
+      </c>
+      <c r="F7" s="18">
+        <v>43354.825324074074</v>
+      </c>
+      <c r="G7" s="18">
+        <v>43390.557476851849</v>
+      </c>
+      <c r="H7" s="18">
+        <v>43398</v>
+      </c>
+      <c r="Q7" s="18">
+        <v>43343</v>
+      </c>
+      <c r="R7" s="18">
+        <v>43402.519155092596</v>
+      </c>
+      <c r="Z7" s="18">
+        <v>43930.941064814811</v>
+      </c>
+    </row>
+    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="N8" s="5">
+        <v>4.06724169668919</v>
+      </c>
+      <c r="S8" s="5">
+        <v>1.09051463433875</v>
+      </c>
+      <c r="U8" s="5">
+        <v>2.9462224209114498</v>
+      </c>
+      <c r="V8" s="5">
+        <v>172.14232527764699</v>
+      </c>
+      <c r="AA8" s="5">
+        <v>120.017472585395</v>
+      </c>
+      <c r="AB8" s="5">
+        <v>20.0102113410668</v>
+      </c>
+      <c r="AC8" s="5">
+        <v>48.803411611048197</v>
+      </c>
+      <c r="AD8" s="5">
+        <v>784.81423725247805</v>
+      </c>
+      <c r="AE8" s="5">
+        <v>2.2063884432990499</v>
+      </c>
+      <c r="AF8" s="5">
+        <v>2108.75804910546</v>
+      </c>
+      <c r="AG8" s="5">
+        <v>30.289531122623298</v>
+      </c>
+      <c r="AH8" s="5">
+        <v>16.606849519201202</v>
+      </c>
+      <c r="AI8" s="5">
+        <v>23.1055828753254</v>
+      </c>
+    </row>
+    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="N9" s="5">
+        <v>1.35775778931876</v>
+      </c>
+      <c r="S9" s="5">
+        <v>0.68446333620384303</v>
+      </c>
+      <c r="U9" s="5">
+        <v>2.7816820201246699</v>
+      </c>
+      <c r="V9" s="5">
+        <v>266.11530624175703</v>
+      </c>
+      <c r="AA9" s="5">
+        <v>182.399261654095</v>
+      </c>
+      <c r="AB9" s="5">
+        <v>15.725962745097</v>
+      </c>
+      <c r="AC9" s="5">
+        <v>10.0160557082775</v>
+      </c>
+      <c r="AD9" s="5">
+        <v>650.54908681232496</v>
+      </c>
+      <c r="AE9" s="5">
+        <v>1.71793297003821</v>
+      </c>
+      <c r="AF9" s="5">
+        <v>3768.6925742180802</v>
+      </c>
+      <c r="AG9" s="5">
+        <v>16.157507511201</v>
+      </c>
+      <c r="AH9" s="5">
+        <v>13.439646076966</v>
+      </c>
+      <c r="AI9" s="5">
+        <v>11.7398389617903</v>
+      </c>
+    </row>
+    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="N10" s="5">
+        <v>1</v>
+      </c>
+      <c r="S10" s="5">
+        <v>1</v>
+      </c>
+      <c r="U10" s="5">
+        <v>0</v>
+      </c>
+      <c r="V10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="5">
+        <v>0.85</v>
+      </c>
+      <c r="AB10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="5">
+        <v>5</v>
+      </c>
+      <c r="AD10" s="5">
+        <v>4</v>
+      </c>
+      <c r="AE10" s="5">
+        <v>1</v>
+      </c>
+      <c r="AF10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG10" s="5">
+        <v>7</v>
+      </c>
+      <c r="AH10" s="5">
+        <v>2</v>
+      </c>
+      <c r="AI10" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A11" s="17">
+        <v>0.25</v>
+      </c>
+      <c r="N11" s="5">
+        <v>4</v>
+      </c>
+      <c r="S11" s="5">
+        <v>1</v>
+      </c>
+      <c r="U11" s="5">
+        <v>1</v>
+      </c>
+      <c r="V11" s="5">
+        <v>60.95</v>
+      </c>
+      <c r="AA11" s="5">
+        <v>39.9</v>
+      </c>
+      <c r="AB11" s="5">
+        <v>13.08</v>
+      </c>
+      <c r="AC11" s="5">
+        <v>42</v>
+      </c>
+      <c r="AD11" s="5">
+        <v>345</v>
+      </c>
+      <c r="AE11" s="5">
+        <v>1</v>
+      </c>
+      <c r="AF11" s="5">
+        <v>300</v>
+      </c>
+      <c r="AG11" s="5">
+        <v>18</v>
+      </c>
+      <c r="AH11" s="5">
+        <v>8</v>
+      </c>
+      <c r="AI11" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A12" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="N12" s="5">
+        <v>5</v>
+      </c>
+      <c r="S12" s="5">
+        <v>1</v>
+      </c>
+      <c r="U12" s="5">
+        <v>2</v>
+      </c>
+      <c r="V12" s="5">
+        <v>108.06</v>
+      </c>
+      <c r="AA12" s="5">
+        <v>74.900000000000006</v>
+      </c>
+      <c r="AB12" s="5">
+        <v>16.32</v>
+      </c>
+      <c r="AC12" s="5">
+        <v>52</v>
+      </c>
+      <c r="AD12" s="5">
+        <v>600</v>
+      </c>
+      <c r="AE12" s="5">
+        <v>1</v>
+      </c>
+      <c r="AF12" s="5">
+        <v>700</v>
+      </c>
+      <c r="AG12" s="5">
+        <v>25</v>
+      </c>
+      <c r="AH12" s="5">
+        <v>13</v>
+      </c>
+      <c r="AI12" s="5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A13" s="17">
+        <v>0.75</v>
+      </c>
+      <c r="N13" s="5">
+        <v>5</v>
+      </c>
+      <c r="S13" s="5">
+        <v>1</v>
+      </c>
+      <c r="U13" s="5">
+        <v>4</v>
+      </c>
+      <c r="V13" s="5">
+        <v>189.37</v>
+      </c>
+      <c r="AA13" s="5">
+        <v>133</v>
+      </c>
+      <c r="AB13" s="5">
+        <v>21.19</v>
+      </c>
+      <c r="AC13" s="5">
+        <v>57</v>
+      </c>
+      <c r="AD13" s="5">
+        <v>983</v>
+      </c>
+      <c r="AE13" s="5">
+        <v>3</v>
+      </c>
+      <c r="AF13" s="5">
+        <v>1800</v>
+      </c>
+      <c r="AG13" s="5">
+        <v>38</v>
+      </c>
+      <c r="AH13" s="5">
+        <v>20</v>
+      </c>
+      <c r="AI13" s="5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="N14" s="5">
+        <v>5</v>
+      </c>
+      <c r="S14" s="5">
+        <v>26</v>
+      </c>
+      <c r="U14" s="5">
+        <v>24</v>
+      </c>
+      <c r="V14" s="5">
+        <v>13664.08</v>
+      </c>
+      <c r="AA14" s="5">
+        <v>6735</v>
+      </c>
+      <c r="AB14" s="5">
+        <v>409.68</v>
+      </c>
+      <c r="AC14" s="5">
+        <v>76</v>
+      </c>
+      <c r="AD14" s="5">
+        <v>3992</v>
+      </c>
+      <c r="AE14" s="5">
+        <v>20</v>
+      </c>
+      <c r="AF14" s="5">
+        <v>40425</v>
+      </c>
+      <c r="AG14" s="5">
+        <v>105</v>
+      </c>
+      <c r="AH14" s="5">
+        <v>105</v>
+      </c>
+      <c r="AI14" s="5">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>